<commit_message>
Updated var, ran completely through. Errors in diathesis regression and SEM model spec (and past)
</commit_message>
<xml_diff>
--- a/missing.xlsx
+++ b/missing.xlsx
@@ -73436,28 +73436,28 @@
         </is>
       </c>
       <c r="B5">
-        <v>4723</v>
+        <v>4724</v>
       </c>
       <c r="C5">
-        <v>0.4639000635189498</v>
+        <v>0.4640135478408129</v>
       </c>
       <c r="D5">
-        <v>0.4639000635189498</v>
+        <v>0.4640135478408129</v>
       </c>
       <c r="E5">
-        <v>0.9972475121744654</v>
+        <v>0.9972480948348857</v>
       </c>
       <c r="F5">
-        <v>0.9462206224857083</v>
+        <v>0.9462320067739204</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0.8164302350201144</v>
+        <v>0.8164690939881456</v>
       </c>
       <c r="I5">
-        <v>0.8164302350201144</v>
+        <v>0.8164690939881456</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -73466,133 +73466,133 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9991530806690663</v>
+        <v>0.9991532599491956</v>
       </c>
       <c r="M5">
-        <v>0.02074952360787635</v>
+        <v>0.02074513124470788</v>
       </c>
       <c r="N5">
-        <v>0.9991530806690663</v>
+        <v>0.9991532599491956</v>
       </c>
       <c r="O5">
-        <v>0.4766038534829558</v>
+        <v>0.4765029635901778</v>
       </c>
       <c r="P5">
-        <v>0.475756934152022</v>
+        <v>0.4756562235393734</v>
       </c>
       <c r="Q5">
-        <v>0.4749100148210883</v>
+        <v>0.474809483488569</v>
       </c>
       <c r="R5">
         <v>1</v>
       </c>
       <c r="S5">
-        <v>0.9978827016726657</v>
+        <v>0.997883149872989</v>
       </c>
       <c r="T5">
         <v>0</v>
       </c>
       <c r="U5">
-        <v>0.7912343849248359</v>
+        <v>0.7912785774767146</v>
       </c>
       <c r="V5">
-        <v>0.6555155621427059</v>
+        <v>0.655376799322608</v>
       </c>
       <c r="W5">
-        <v>0.4795680711412238</v>
+        <v>0.4796782387806943</v>
       </c>
       <c r="X5">
-        <v>0.8138894770273132</v>
+        <v>0.8137171888230313</v>
       </c>
       <c r="Y5">
-        <v>0.4770273131484226</v>
+        <v>0.47692633361558</v>
       </c>
       <c r="Z5">
-        <v>0.4751217446538217</v>
+        <v>0.4750211685012701</v>
       </c>
       <c r="AA5">
-        <v>0.2125767520643659</v>
+        <v>0.2125317527519052</v>
       </c>
       <c r="AB5">
-        <v>0.649163667160703</v>
+        <v>0.6492379339542761</v>
       </c>
       <c r="AC5">
-        <v>0.7154351048062672</v>
+        <v>0.7154953429297206</v>
       </c>
       <c r="AD5">
-        <v>0.7010374761803938</v>
+        <v>0.7011007620660458</v>
       </c>
       <c r="AE5">
-        <v>0.8947702731314843</v>
+        <v>0.8947925486875529</v>
       </c>
       <c r="AF5">
-        <v>0.695744230362058</v>
+        <v>0.6958086367485182</v>
       </c>
       <c r="AG5">
-        <v>0.7317383019267415</v>
+        <v>0.7317950889077053</v>
       </c>
       <c r="AH5">
-        <v>0.8229938598348507</v>
+        <v>0.8230313293818797</v>
       </c>
       <c r="AI5">
-        <v>0.4763921236502223</v>
+        <v>0.4762912785774767</v>
       </c>
       <c r="AJ5">
-        <v>0.9995765403345331</v>
+        <v>0.9995766299745978</v>
       </c>
       <c r="AK5">
-        <v>0.9989413508363328</v>
+        <v>0.9989415749364945</v>
       </c>
       <c r="AL5">
-        <v>0.9928011856870633</v>
+        <v>0.9928027095681625</v>
       </c>
       <c r="AM5">
-        <v>0.7537582045310184</v>
+        <v>0.7538103302286198</v>
       </c>
       <c r="AN5">
         <v>1</v>
       </c>
       <c r="AO5">
-        <v>0.9911073470251959</v>
+        <v>0.9911092294665538</v>
       </c>
       <c r="AP5">
-        <v>0.982849883548592</v>
+        <v>0.9828535139712108</v>
       </c>
       <c r="AQ5">
-        <v>0.6961676900275249</v>
+        <v>0.6962320067739204</v>
       </c>
       <c r="AR5">
-        <v>0.9989413508363328</v>
+        <v>0.9989415749364945</v>
       </c>
       <c r="AS5">
-        <v>0.8545416049121322</v>
+        <v>0.8543607112616427</v>
       </c>
       <c r="AT5">
         <v>1</v>
       </c>
       <c r="AU5">
-        <v>0.915731526572094</v>
+        <v>0.915749364944962</v>
       </c>
       <c r="AV5">
-        <v>0.8088079610417108</v>
+        <v>0.8086367485182049</v>
       </c>
       <c r="AW5">
-        <v>0.8240525089985179</v>
+        <v>0.8238780694326842</v>
       </c>
       <c r="AX5">
-        <v>0.8458606817700614</v>
+        <v>0.8456816257408976</v>
       </c>
       <c r="AY5">
-        <v>0.9993648105017997</v>
+        <v>0.9993649449618967</v>
       </c>
       <c r="AZ5">
-        <v>0.5809866610205378</v>
+        <v>0.5810753598645216</v>
       </c>
       <c r="BA5">
-        <v>0.9944950243489308</v>
+        <v>0.9944961896697714</v>
       </c>
       <c r="BB5">
-        <v>0.9923777260215965</v>
+        <v>0.9923793395427604</v>
       </c>
       <c r="BC5">
         <v>1</v>
@@ -73601,31 +73601,31 @@
         <v>1</v>
       </c>
       <c r="BE5">
-        <v>0.9997882701672666</v>
+        <v>0.9997883149872989</v>
       </c>
       <c r="BF5">
-        <v>0.9993648105017997</v>
+        <v>0.9993649449618967</v>
       </c>
       <c r="BG5">
-        <v>0.9822146940503917</v>
+        <v>0.9822184589331076</v>
       </c>
       <c r="BH5">
         <v>1</v>
       </c>
       <c r="BI5">
-        <v>0.7997035782341732</v>
+        <v>0.7997459779847587</v>
       </c>
       <c r="BJ5">
-        <v>0.4802032606394241</v>
+        <v>0.4803132938187976</v>
       </c>
       <c r="BK5">
-        <v>0.4804149904721575</v>
+        <v>0.4805249788314988</v>
       </c>
       <c r="BL5">
-        <v>0.9923777260215965</v>
+        <v>0.9923793395427604</v>
       </c>
       <c r="BM5">
-        <v>0.4031336015244548</v>
+        <v>0.4030482641828959</v>
       </c>
     </row>
     <row r="6">
@@ -74232,28 +74232,28 @@
         </is>
       </c>
       <c r="B9">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C9">
-        <v>0.4</v>
+        <v>0.3966480446927375</v>
       </c>
       <c r="D9">
-        <v>0.5944444444444444</v>
+        <v>0.5921787709497207</v>
       </c>
       <c r="E9">
-        <v>0.9944444444444445</v>
+        <v>0.994413407821229</v>
       </c>
       <c r="F9">
-        <v>0.9166666666666666</v>
+        <v>0.9162011173184358</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0.8777777777777778</v>
+        <v>0.8770949720670391</v>
       </c>
       <c r="I9">
-        <v>0.8777777777777778</v>
+        <v>0.8770949720670391</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -74265,130 +74265,130 @@
         <v>1</v>
       </c>
       <c r="M9">
-        <v>0.005555555555555556</v>
+        <v>0.00558659217877095</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9">
-        <v>0.6055555555555555</v>
+        <v>0.6089385474860335</v>
       </c>
       <c r="P9">
-        <v>0.5888888888888889</v>
+        <v>0.5921787709497207</v>
       </c>
       <c r="Q9">
-        <v>0.5888888888888889</v>
+        <v>0.5921787709497207</v>
       </c>
       <c r="R9">
         <v>1</v>
       </c>
       <c r="S9">
-        <v>0.9944444444444445</v>
+        <v>0.994413407821229</v>
       </c>
       <c r="T9">
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0.85</v>
+        <v>0.8491620111731844</v>
       </c>
       <c r="V9">
-        <v>0.6666666666666666</v>
+        <v>0.6703910614525139</v>
       </c>
       <c r="W9">
-        <v>0.4222222222222222</v>
+        <v>0.4189944134078212</v>
       </c>
       <c r="X9">
-        <v>0.8555555555555555</v>
+        <v>0.8603351955307262</v>
       </c>
       <c r="Y9">
-        <v>0.6055555555555555</v>
+        <v>0.6089385474860335</v>
       </c>
       <c r="Z9">
-        <v>0.6055555555555555</v>
+        <v>0.6089385474860335</v>
       </c>
       <c r="AA9">
-        <v>0.2722222222222222</v>
+        <v>0.2737430167597765</v>
       </c>
       <c r="AB9">
-        <v>0.5722222222222222</v>
+        <v>0.5698324022346368</v>
       </c>
       <c r="AC9">
-        <v>0.5944444444444444</v>
+        <v>0.5921787709497207</v>
       </c>
       <c r="AD9">
-        <v>0.5944444444444444</v>
+        <v>0.5921787709497207</v>
       </c>
       <c r="AE9">
-        <v>0.8444444444444444</v>
+        <v>0.8435754189944135</v>
       </c>
       <c r="AF9">
-        <v>0.5555555555555556</v>
+        <v>0.553072625698324</v>
       </c>
       <c r="AG9">
-        <v>0.6444444444444445</v>
+        <v>0.6424581005586593</v>
       </c>
       <c r="AH9">
-        <v>0.8666666666666667</v>
+        <v>0.8659217877094972</v>
       </c>
       <c r="AI9">
-        <v>0.6</v>
+        <v>0.6033519553072626</v>
       </c>
       <c r="AJ9">
         <v>1</v>
       </c>
       <c r="AK9">
-        <v>0.9944444444444445</v>
+        <v>0.994413407821229</v>
       </c>
       <c r="AL9">
-        <v>0.9888888888888889</v>
+        <v>0.9888268156424581</v>
       </c>
       <c r="AM9">
-        <v>0.8222222222222222</v>
+        <v>0.8212290502793296</v>
       </c>
       <c r="AN9">
         <v>1</v>
       </c>
       <c r="AO9">
-        <v>0.9833333333333333</v>
+        <v>0.9832402234636871</v>
       </c>
       <c r="AP9">
-        <v>0.9611111111111111</v>
+        <v>0.9608938547486033</v>
       </c>
       <c r="AQ9">
-        <v>0.7555555555555555</v>
+        <v>0.7541899441340782</v>
       </c>
       <c r="AR9">
         <v>1</v>
       </c>
       <c r="AS9">
-        <v>0.7944444444444444</v>
+        <v>0.7988826815642458</v>
       </c>
       <c r="AT9">
         <v>1</v>
       </c>
       <c r="AU9">
-        <v>0.9277777777777778</v>
+        <v>0.9273743016759777</v>
       </c>
       <c r="AV9">
-        <v>0.7388888888888889</v>
+        <v>0.7430167597765364</v>
       </c>
       <c r="AW9">
-        <v>0.7388888888888889</v>
+        <v>0.7430167597765364</v>
       </c>
       <c r="AX9">
-        <v>0.7888888888888889</v>
+        <v>0.7932960893854749</v>
       </c>
       <c r="AY9">
-        <v>0.9944444444444445</v>
+        <v>0.994413407821229</v>
       </c>
       <c r="AZ9">
-        <v>0.6722222222222223</v>
+        <v>0.6703910614525139</v>
       </c>
       <c r="BA9">
-        <v>0.9833333333333333</v>
+        <v>0.9832402234636871</v>
       </c>
       <c r="BB9">
-        <v>0.9944444444444445</v>
+        <v>0.994413407821229</v>
       </c>
       <c r="BC9">
         <v>1</v>
@@ -74403,25 +74403,25 @@
         <v>1</v>
       </c>
       <c r="BG9">
-        <v>0.95</v>
+        <v>0.9497206703910615</v>
       </c>
       <c r="BH9">
         <v>1</v>
       </c>
       <c r="BI9">
-        <v>0.8111111111111111</v>
+        <v>0.8100558659217877</v>
       </c>
       <c r="BJ9">
-        <v>0.4222222222222222</v>
+        <v>0.4189944134078212</v>
       </c>
       <c r="BK9">
-        <v>0.4222222222222222</v>
+        <v>0.4189944134078212</v>
       </c>
       <c r="BL9">
-        <v>0.9944444444444445</v>
+        <v>0.994413407821229</v>
       </c>
       <c r="BM9">
-        <v>0.5611111111111111</v>
+        <v>0.5642458100558659</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
EFA now working with cut-off component line. Still need to fix OR regressions on dia, env.
</commit_message>
<xml_diff>
--- a/missing.xlsx
+++ b/missing.xlsx
@@ -781,7 +781,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995158389818786</v>
+        <v>0.08286069995850048</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -978,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9993896484375</v>
+        <v>0.183349609375</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1341,7 +1341,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BM4"/>
+  <dimension ref="A1:BM3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1676,31 +1676,31 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>40202</v>
+        <v>5427</v>
       </c>
       <c r="C2">
-        <v>0.4959454753494851</v>
+        <v>0.4975124378109453</v>
       </c>
       <c r="D2">
-        <v>0.3993582408835381</v>
+        <v>0.6023585774829556</v>
       </c>
       <c r="E2">
-        <v>0.9972886921048704</v>
+        <v>0.9985258890731528</v>
       </c>
       <c r="F2">
-        <v>0.943982886423561</v>
+        <v>0.9386401326699834</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.7776230038306552</v>
+        <v>0.8131564400221116</v>
       </c>
       <c r="I2">
-        <v>0.7776230038306552</v>
+        <v>0.8131564400221116</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1712,553 +1712,356 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>0.01529774638077708</v>
+        <v>0.01013451262207481</v>
       </c>
       <c r="N2">
-        <v>0.9989801502412815</v>
+        <v>0.9990786806707205</v>
       </c>
       <c r="O2">
-        <v>0.5114173424207751</v>
+        <v>0.556661138750691</v>
       </c>
       <c r="P2">
-        <v>0.5105467389682106</v>
+        <v>0.554818500092132</v>
       </c>
       <c r="Q2">
-        <v>0.5101984975871847</v>
+        <v>0.5551870278238438</v>
       </c>
       <c r="R2">
         <v>1</v>
       </c>
       <c r="S2">
-        <v>0.9968409531864086</v>
+        <v>0.9972360420121614</v>
       </c>
       <c r="T2">
         <v>0</v>
       </c>
       <c r="U2">
-        <v>0.7479229889060246</v>
+        <v>0.8092868988391376</v>
       </c>
       <c r="V2">
-        <v>0.6459380130341774</v>
+        <v>0.6112032430440391</v>
       </c>
       <c r="W2">
-        <v>0.5506939953236157</v>
+        <v>0.5463423622627602</v>
       </c>
       <c r="X2">
-        <v>0.7772250136809113</v>
+        <v>0.8111295374976967</v>
       </c>
       <c r="Y2">
-        <v>0.5111437241928263</v>
+        <v>0.5572139303482587</v>
       </c>
       <c r="Z2">
-        <v>0.5106711108900055</v>
+        <v>0.5561083471531233</v>
       </c>
       <c r="AA2">
-        <v>0.1766827521018855</v>
+        <v>0.3080891837110742</v>
       </c>
       <c r="AB2">
-        <v>0.6719317446893189</v>
+        <v>0.5651372765800626</v>
       </c>
       <c r="AC2">
-        <v>0.7227003631660116</v>
+        <v>0.5391560714943799</v>
       </c>
       <c r="AD2">
-        <v>0.7042186955872842</v>
+        <v>0.5316012529942878</v>
       </c>
       <c r="AE2">
-        <v>0.8868961743196856</v>
+        <v>0.8625391560714943</v>
       </c>
       <c r="AF2">
-        <v>0.6939207004626635</v>
+        <v>0.5043302008476138</v>
       </c>
       <c r="AG2">
-        <v>0.7191184518183175</v>
+        <v>0.5957250783121429</v>
       </c>
       <c r="AH2">
-        <v>0.7845132082980947</v>
+        <v>0.8170259812050856</v>
       </c>
       <c r="AI2">
-        <v>0.5104969901994926</v>
+        <v>0.5557398194214115</v>
       </c>
       <c r="AJ2">
-        <v>0.9995025123128203</v>
+        <v>0.9998157361341441</v>
       </c>
       <c r="AK2">
-        <v>0.9993035172379484</v>
+        <v>0.9996314722682882</v>
       </c>
       <c r="AL2">
-        <v>0.9932839162230734</v>
+        <v>0.9926294453657638</v>
       </c>
       <c r="AM2">
-        <v>0.7127257350380578</v>
+        <v>0.7962041643633684</v>
       </c>
       <c r="AN2">
         <v>1</v>
       </c>
       <c r="AO2">
-        <v>0.9917665787771752</v>
+        <v>0.9900497512437811</v>
       </c>
       <c r="AP2">
-        <v>0.9831849161733247</v>
+        <v>0.9854431545973834</v>
       </c>
       <c r="AQ2">
-        <v>0.7113327695139545</v>
+        <v>0.7589828634604754</v>
       </c>
       <c r="AR2">
-        <v>0.9992537684692304</v>
+        <v>0.9994472084024323</v>
       </c>
       <c r="AS2">
-        <v>0.8400825829560719</v>
+        <v>0.765616362631288</v>
       </c>
       <c r="AT2">
         <v>1</v>
       </c>
       <c r="AU2">
-        <v>0.9079399034873887</v>
+        <v>0.8719366132301456</v>
       </c>
       <c r="AV2">
-        <v>0.7880453708770708</v>
+        <v>0.6622443338861249</v>
       </c>
       <c r="AW2">
-        <v>0.8012536689716929</v>
+        <v>0.6963331490694675</v>
       </c>
       <c r="AX2">
-        <v>0.8310034326650415</v>
+        <v>0.7372397272894785</v>
       </c>
       <c r="AY2">
-        <v>0.9993532660066663</v>
+        <v>0.9992629445365764</v>
       </c>
       <c r="AZ2">
-        <v>0.5354211233271976</v>
+        <v>0.7880965542657085</v>
       </c>
       <c r="BA2">
-        <v>0.9938311526789712</v>
+        <v>0.9937350285608992</v>
       </c>
       <c r="BB2">
-        <v>0.9930102979951246</v>
+        <v>0.994103556292611</v>
       </c>
       <c r="BC2">
-        <v>0.9988806527038456</v>
+        <v>0.9988944168048646</v>
       </c>
       <c r="BD2">
         <v>1</v>
       </c>
       <c r="BE2">
-        <v>0.9997512561564101</v>
+        <v>0.9996314722682882</v>
       </c>
       <c r="BF2">
-        <v>0.9987065320133327</v>
+        <v>0.9988944168048646</v>
       </c>
       <c r="BG2">
-        <v>0.9779612954579374</v>
+        <v>0.9719918923899024</v>
       </c>
       <c r="BH2">
         <v>1</v>
       </c>
       <c r="BI2">
-        <v>0.7594398288642356</v>
+        <v>0.7921503593145384</v>
       </c>
       <c r="BJ2">
-        <v>0.5511417342420775</v>
+        <v>0.5465266261286161</v>
       </c>
       <c r="BK2">
-        <v>0.5508929903984876</v>
+        <v>0.5459738345310484</v>
       </c>
       <c r="BL2">
-        <v>0.9926620566140988</v>
+        <v>0.9946563478901788</v>
       </c>
       <c r="BM2">
-        <v>0.397691657131486</v>
+        <v>0.6065966463976414</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>1</v>
-      </c>
       <c r="B3">
-        <v>5427</v>
+        <v>40227</v>
       </c>
       <c r="C3">
-        <v>0.4975124378109453</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.6023585774829556</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.9985258890731528</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.9386401326699834</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0.8131564400221116</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.8131564400221116</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>0.01013451262207481</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>0.9990786806707205</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>0.556661138750691</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0.554818500092132</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>0.5551870278238438</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>0.9972360420121614</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <v>0</v>
       </c>
       <c r="U3">
-        <v>0.8092868988391376</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>0.6112032430440391</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>0.5463423622627602</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>0.8111295374976967</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <v>0.5572139303482587</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <v>0.5561083471531233</v>
+        <v>0</v>
       </c>
       <c r="AA3">
-        <v>0.3080891837110742</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <v>0.5651372765800626</v>
+        <v>0</v>
       </c>
       <c r="AC3">
-        <v>0.5391560714943799</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <v>0.5316012529942878</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <v>0.8625391560714943</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <v>0.5043302008476138</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <v>0.5957250783121429</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <v>0.8170259812050856</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <v>0.5557398194214115</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
-        <v>0.9998157361341441</v>
+        <v>0</v>
       </c>
       <c r="AK3">
-        <v>0.9996314722682882</v>
+        <v>0</v>
       </c>
       <c r="AL3">
-        <v>0.9926294453657638</v>
+        <v>0</v>
       </c>
       <c r="AM3">
-        <v>0.7962041643633684</v>
+        <v>0</v>
       </c>
       <c r="AN3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO3">
-        <v>0.9900497512437811</v>
+        <v>0</v>
       </c>
       <c r="AP3">
-        <v>0.9854431545973834</v>
+        <v>0</v>
       </c>
       <c r="AQ3">
-        <v>0.7589828634604754</v>
+        <v>0</v>
       </c>
       <c r="AR3">
-        <v>0.9994472084024323</v>
+        <v>0</v>
       </c>
       <c r="AS3">
-        <v>0.765616362631288</v>
+        <v>0</v>
       </c>
       <c r="AT3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU3">
-        <v>0.8719366132301456</v>
+        <v>0</v>
       </c>
       <c r="AV3">
-        <v>0.6622443338861249</v>
+        <v>0</v>
       </c>
       <c r="AW3">
-        <v>0.6963331490694675</v>
+        <v>0</v>
       </c>
       <c r="AX3">
-        <v>0.7372397272894785</v>
+        <v>0</v>
       </c>
       <c r="AY3">
-        <v>0.9992629445365764</v>
+        <v>0</v>
       </c>
       <c r="AZ3">
-        <v>0.7880965542657085</v>
+        <v>0</v>
       </c>
       <c r="BA3">
-        <v>0.9937350285608992</v>
+        <v>0</v>
       </c>
       <c r="BB3">
-        <v>0.994103556292611</v>
+        <v>0</v>
       </c>
       <c r="BC3">
-        <v>0.9988944168048646</v>
+        <v>0</v>
       </c>
       <c r="BD3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE3">
-        <v>0.9996314722682882</v>
+        <v>0</v>
       </c>
       <c r="BF3">
-        <v>0.9988944168048646</v>
+        <v>0</v>
       </c>
       <c r="BG3">
-        <v>0.9719918923899024</v>
+        <v>0</v>
       </c>
       <c r="BH3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI3">
-        <v>0.7921503593145384</v>
+        <v>0</v>
       </c>
       <c r="BJ3">
-        <v>0.5465266261286161</v>
+        <v>0</v>
       </c>
       <c r="BK3">
-        <v>0.5459738345310484</v>
+        <v>0</v>
       </c>
       <c r="BL3">
-        <v>0.9946563478901788</v>
+        <v>0</v>
       </c>
       <c r="BM3">
-        <v>0.6065966463976414</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4">
-        <v>25</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
-      </c>
-      <c r="AJ4">
-        <v>0</v>
-      </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
-      <c r="AM4">
-        <v>0</v>
-      </c>
-      <c r="AN4">
-        <v>0</v>
-      </c>
-      <c r="AO4">
-        <v>0</v>
-      </c>
-      <c r="AP4">
-        <v>0</v>
-      </c>
-      <c r="AQ4">
-        <v>0</v>
-      </c>
-      <c r="AR4">
-        <v>0</v>
-      </c>
-      <c r="AS4">
-        <v>0</v>
-      </c>
-      <c r="AT4">
-        <v>0</v>
-      </c>
-      <c r="AU4">
-        <v>0</v>
-      </c>
-      <c r="AV4">
-        <v>0</v>
-      </c>
-      <c r="AW4">
-        <v>0</v>
-      </c>
-      <c r="AX4">
-        <v>0</v>
-      </c>
-      <c r="AY4">
-        <v>0</v>
-      </c>
-      <c r="AZ4">
-        <v>0</v>
-      </c>
-      <c r="BA4">
-        <v>0</v>
-      </c>
-      <c r="BB4">
-        <v>0</v>
-      </c>
-      <c r="BC4">
-        <v>0</v>
-      </c>
-      <c r="BD4">
-        <v>0</v>
-      </c>
-      <c r="BE4">
-        <v>0</v>
-      </c>
-      <c r="BF4">
-        <v>0</v>
-      </c>
-      <c r="BG4">
-        <v>0</v>
-      </c>
-      <c r="BH4">
-        <v>0</v>
-      </c>
-      <c r="BI4">
-        <v>0</v>
-      </c>
-      <c r="BJ4">
-        <v>0</v>
-      </c>
-      <c r="BK4">
-        <v>0</v>
-      </c>
-      <c r="BL4">
-        <v>0</v>
-      </c>
-      <c r="BM4">
         <v>0</v>
       </c>
     </row>
@@ -2637,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0.07102272727272728</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -2834,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.0872093023255814</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -3031,7 +2834,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0.0273972602739726</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -3228,7 +3031,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0.1052631578947368</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -3425,7 +3228,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.2173913043478261</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -3622,7 +3425,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -3819,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -4016,7 +3819,7 @@
         <v>1</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -4410,7 +4213,7 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -4607,7 +4410,7 @@
         <v>1</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -4804,7 +4607,7 @@
         <v>1</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -5001,7 +4804,7 @@
         <v>1</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <v>1</v>
@@ -5734,7 +5537,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9992033988316517</v>
+        <v>0.1255974508762613</v>
       </c>
       <c r="M2">
         <v>0.02124269782262347</v>
@@ -5933,7 +5736,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9992894573230304</v>
+        <v>0.1215027977617906</v>
       </c>
       <c r="M3">
         <v>0.01749711342037481</v>
@@ -6132,7 +5935,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9995059288537549</v>
+        <v>0.1207180500658762</v>
       </c>
       <c r="M4">
         <v>0.01688076416337286</v>
@@ -6331,7 +6134,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9996957249353415</v>
+        <v>0.1179065875551498</v>
       </c>
       <c r="M5">
         <v>0.01369237790963031</v>
@@ -6530,7 +6333,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9995332555425904</v>
+        <v>0.1091015169194866</v>
       </c>
       <c r="M6">
         <v>0.008401400233372229</v>
@@ -6729,7 +6532,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.9993932038834952</v>
+        <v>0.122876213592233</v>
       </c>
       <c r="M7">
         <v>0.007888349514563107</v>
@@ -7462,7 +7265,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.998920474991004</v>
+        <v>0.1144296509535804</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -7661,7 +7464,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9995613554117776</v>
+        <v>0.1188726834082685</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -7860,7 +7663,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9992691127028213</v>
+        <v>0.1286361643034644</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -8059,7 +7862,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9996102883865939</v>
+        <v>0.1391270459859704</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -8258,7 +8061,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.1627296587926509</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -8457,7 +8260,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.1751633986928104</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -9190,7 +8993,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0.1692913385826772</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -9389,7 +9192,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9994036970781157</v>
+        <v>0.1413237924865832</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -9588,7 +9391,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0.1281576288312563</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -9787,7 +9590,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9991177767975298</v>
+        <v>0.1228495809439788</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -9986,7 +9789,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9995160509759639</v>
+        <v>0.1216325213744152</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -10185,7 +9988,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.998</v>
+        <v>0.1035</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -10918,7 +10721,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994131455399061</v>
+        <v>0.1470070422535211</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -11117,7 +10920,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9996911673872761</v>
+        <v>0.1280111179740581</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -11316,7 +11119,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9998403830806065</v>
+        <v>0.1158818834796488</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -11515,7 +11318,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9985043374214777</v>
+        <v>0.13221657194137</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -11714,7 +11517,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9990445859872611</v>
+        <v>0.1251592356687898</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -11913,7 +11716,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.1348066298342541</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -12646,7 +12449,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995672494374243</v>
+        <v>0.08957936645317639</v>
       </c>
       <c r="M2">
         <v>0.01276614159598407</v>
@@ -12845,7 +12648,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9996074326092645</v>
+        <v>0.1044229259356189</v>
       </c>
       <c r="M3">
         <v>0.04239727819942424</v>
@@ -13044,7 +12847,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.99893219434063</v>
+        <v>0.1494927923117993</v>
       </c>
       <c r="M4">
         <v>0.005161060686954974</v>
@@ -13243,7 +13046,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9997637609260571</v>
+        <v>0.1691471769430664</v>
       </c>
       <c r="M5">
         <v>0.003543586109142452</v>
@@ -13442,7 +13245,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9992281965526113</v>
+        <v>0.1950090043735529</v>
       </c>
       <c r="M6">
         <v>0.0007718034473887317</v>
@@ -13641,7 +13444,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.9987325728770595</v>
+        <v>0.2179974651457541</v>
       </c>
       <c r="M7">
         <v>0.001267427122940431</v>
@@ -13840,7 +13643,7 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>0.9958677685950413</v>
+        <v>0.2190082644628099</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -14039,7 +13842,7 @@
         <v>1</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0.1492537313432836</v>
       </c>
       <c r="M9">
         <v>0.02238805970149254</v>
@@ -14578,7 +14381,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9977578475336323</v>
+        <v>0.1255605381165919</v>
       </c>
       <c r="M2">
         <v>0.01569506726457399</v>
@@ -14777,7 +14580,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9995483288166215</v>
+        <v>0.1043360433604336</v>
       </c>
       <c r="M3">
         <v>0.01580849141824752</v>
@@ -14976,7 +14779,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9994106713812956</v>
+        <v>0.1073031415748674</v>
       </c>
       <c r="M4">
         <v>0.01582120676367922</v>
@@ -15175,7 +14978,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9994783175741767</v>
+        <v>0.1345288555591783</v>
       </c>
       <c r="M5">
         <v>0.01258558852298663</v>
@@ -15374,7 +15177,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.999691738594328</v>
+        <v>0.1430332922318126</v>
       </c>
       <c r="M6">
         <v>0.01541307028360049</v>
@@ -16641,7 +16444,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9992202729044835</v>
+        <v>0.06559454191033139</v>
       </c>
       <c r="M2">
         <v>0.02212475633528265</v>
@@ -16840,7 +16643,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9996731492073868</v>
+        <v>0.1346625265566269</v>
       </c>
       <c r="M3">
         <v>0.01814021899003105</v>
@@ -17039,7 +16842,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9997661365762395</v>
+        <v>0.2018241347053321</v>
       </c>
       <c r="M4">
         <v>0.01169317118802619</v>
@@ -17238,7 +17041,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9974779319041615</v>
+        <v>0.2421185372005044</v>
       </c>
       <c r="M5">
         <v>0.01324085750315259</v>
@@ -17969,7 +17772,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9996943765281173</v>
+        <v>0.148838630806846</v>
       </c>
       <c r="M2">
         <v>0.01491442542787286</v>
@@ -18166,7 +17969,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9986545576858392</v>
+        <v>0.2805247225025227</v>
       </c>
       <c r="M3">
         <v>0.01009081735620585</v>
@@ -18897,7 +18700,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9992834231897905</v>
+        <v>0.113185013307855</v>
       </c>
       <c r="M2">
         <v>0.01866511977069542</v>
@@ -19630,7 +19433,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995431703974418</v>
+        <v>0.1587482868889904</v>
       </c>
       <c r="M2">
         <v>0.003883051621745089</v>
@@ -19829,7 +19632,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9996893445169307</v>
+        <v>0.1309412861136999</v>
       </c>
       <c r="M3">
         <v>0.005591798695246971</v>
@@ -20028,7 +19831,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9995361781076066</v>
+        <v>0.1156462585034014</v>
       </c>
       <c r="M4">
         <v>0.004174397031539889</v>
@@ -20227,7 +20030,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9997074312463429</v>
+        <v>0.1009362200117028</v>
       </c>
       <c r="M5">
         <v>0.006143943826799298</v>
@@ -20426,7 +20229,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9992732558139535</v>
+        <v>0.08902616279069768</v>
       </c>
       <c r="M6">
         <v>0.005813953488372093</v>
@@ -20625,7 +20428,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.9987966305655837</v>
+        <v>0.05354993983152828</v>
       </c>
       <c r="M7">
         <v>0.01083032490974729</v>
@@ -21356,7 +21159,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9993328885923949</v>
+        <v>0.1436513231042917</v>
       </c>
       <c r="M2">
         <v>0.01867911941294196</v>
@@ -21553,7 +21356,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9994138599576176</v>
+        <v>0.1110960818792552</v>
       </c>
       <c r="M3">
         <v>0.01826051670499121</v>
@@ -22286,7 +22089,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994588326246617</v>
+        <v>0.08341708542713568</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -22485,7 +22288,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9996995643683341</v>
+        <v>0.1589304491512693</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -22684,7 +22487,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9989963198394112</v>
+        <v>0.2054198728671797</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -22883,7 +22686,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9986187845303868</v>
+        <v>0.281767955801105</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -23082,7 +22885,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.2696629213483146</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -23281,7 +23084,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.2038834951456311</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -24014,7 +23817,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9991776315789473</v>
+        <v>0.1261748120300752</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -24213,7 +24016,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9997750534248117</v>
+        <v>0.1195591047126307</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -24412,7 +24215,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9995011224744326</v>
+        <v>0.1359441257171364</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -24611,7 +24414,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0.1492932862190813</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -24810,7 +24613,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9970760233918129</v>
+        <v>0.1608187134502924</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -25009,7 +24812,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.1711711711711712</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -25742,7 +25545,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995443672400045</v>
+        <v>0.1904544936780954</v>
       </c>
       <c r="M2">
         <v>0.006492766829935073</v>
@@ -26473,7 +26276,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995698924731182</v>
+        <v>0.09100358422939069</v>
       </c>
       <c r="M2">
         <v>0.02168458781362007</v>
@@ -26670,7 +26473,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.2408759124087591</v>
       </c>
       <c r="M3">
         <v>0.002737226277372263</v>
@@ -27403,7 +27206,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994715286035143</v>
+        <v>0.08690051525961158</v>
       </c>
       <c r="M2">
         <v>0.01608534813053243</v>
@@ -27602,7 +27405,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.1715116279069767</v>
       </c>
       <c r="M3">
         <v>0.008720930232558139</v>
@@ -28335,7 +28138,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994715286035143</v>
+        <v>0.08690051525961158</v>
       </c>
       <c r="M2">
         <v>0.01608534813053243</v>
@@ -28534,7 +28337,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.2713675213675213</v>
       </c>
       <c r="M3">
         <v>0.00641025641025641</v>
@@ -29267,7 +29070,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994715286035143</v>
+        <v>0.08690051525961158</v>
       </c>
       <c r="M2">
         <v>0.01608534813053243</v>
@@ -29466,7 +29269,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9995040174585854</v>
+        <v>0.2033528419799623</v>
       </c>
       <c r="M3">
         <v>0.008630096220613035</v>
@@ -30199,7 +30002,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.999358504398827</v>
+        <v>0.05388563049853373</v>
       </c>
       <c r="M2">
         <v>0.01603739002932551</v>
@@ -30398,7 +30201,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9995508501764517</v>
+        <v>0.1054218800128329</v>
       </c>
       <c r="M3">
         <v>0.01539942252165544</v>
@@ -30597,7 +30400,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9997219905476786</v>
+        <v>0.1489203966268186</v>
       </c>
       <c r="M4">
         <v>0.01334445371142619</v>
@@ -30796,7 +30599,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9990301854770275</v>
+        <v>0.1916595951024367</v>
       </c>
       <c r="M5">
         <v>0.01345617650624318</v>
@@ -31529,7 +31332,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994715286035143</v>
+        <v>0.08690051525961158</v>
       </c>
       <c r="M2">
         <v>0.01608534813053243</v>
@@ -31728,7 +31531,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.2834224598930482</v>
       </c>
       <c r="M3">
         <v>0.01336898395721925</v>
@@ -32461,7 +32264,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994715286035143</v>
+        <v>0.08690051525961158</v>
       </c>
       <c r="M2">
         <v>0.01608534813053243</v>
@@ -32660,7 +32463,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.3197026022304832</v>
       </c>
       <c r="M3">
         <v>0.01699415825809878</v>
@@ -33393,7 +33196,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9993789977022915</v>
+        <v>0.1097621561199776</v>
       </c>
       <c r="M2">
         <v>0.0191889709991927</v>
@@ -33592,7 +33395,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9994721562417525</v>
+        <v>0.2372657693322776</v>
       </c>
       <c r="M3">
         <v>0.01266825019794141</v>
@@ -34325,7 +34128,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9987536352305775</v>
+        <v>0.188616535105941</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -34524,7 +34327,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9988119988119988</v>
+        <v>0.1621621621621622</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -34723,7 +34526,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9998142299832807</v>
+        <v>0.1359836522385287</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -34922,7 +34725,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9994408201304753</v>
+        <v>0.1232059645852749</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -35121,7 +34924,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9996481970096746</v>
+        <v>0.08988566402814424</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -35320,7 +35123,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.08327137546468401</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -36053,7 +35856,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9992205767731879</v>
+        <v>0.1802416212003118</v>
       </c>
       <c r="M2">
         <v>0.01052221356196415</v>
@@ -36252,7 +36055,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9994212404745828</v>
+        <v>0.1429536027780457</v>
       </c>
       <c r="M3">
         <v>0.0126362496382753</v>
@@ -36451,7 +36254,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9993298403801633</v>
+        <v>0.1086267820153528</v>
       </c>
       <c r="M4">
         <v>0.01486535884001462</v>
@@ -36650,7 +36453,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9996061053668144</v>
+        <v>0.09030034465780404</v>
       </c>
       <c r="M5">
         <v>0.01792220580994584</v>
@@ -36849,7 +36652,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.08948106591865358</v>
       </c>
       <c r="M6">
         <v>0.01654978962131837</v>
@@ -37582,7 +37385,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9993438320209974</v>
+        <v>0.1824146981627296</v>
       </c>
       <c r="M2">
         <v>0.01706036745406824</v>
@@ -37781,7 +37584,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.999179116729601</v>
+        <v>0.1436545723198161</v>
       </c>
       <c r="M3">
         <v>0.01362666228862256</v>
@@ -37980,7 +37783,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9991333737758905</v>
+        <v>0.1163012392755005</v>
       </c>
       <c r="M4">
         <v>0.0156859346563827</v>
@@ -38179,7 +37982,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9996028856972665</v>
+        <v>0.1081474617777484</v>
       </c>
       <c r="M5">
         <v>0.01542127208948309</v>
@@ -38378,7 +38181,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9997966859814984</v>
+        <v>0.103486835417302</v>
       </c>
       <c r="M6">
         <v>0.01230049811934533</v>
@@ -39111,7 +38914,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -39310,7 +39113,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -39509,7 +39312,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0.2692307692307692</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -39708,7 +39511,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -39907,7 +39710,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -40106,7 +39909,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.1842105263157895</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -40305,7 +40108,7 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0.09836065573770492</v>
       </c>
       <c r="M8">
         <v>0.03278688524590164</v>
@@ -40504,7 +40307,7 @@
         <v>1</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="M9">
         <v>0.02083333333333333</v>
@@ -40703,7 +40506,7 @@
         <v>1</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>0.2261904761904762</v>
       </c>
       <c r="M10">
         <v>0.0119047619047619</v>
@@ -40902,7 +40705,7 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0.2463768115942029</v>
       </c>
       <c r="M11">
         <v>0.01449275362318841</v>
@@ -41101,7 +40904,7 @@
         <v>1</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0.2345679012345679</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -41300,7 +41103,7 @@
         <v>1</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0.1826086956521739</v>
       </c>
       <c r="M13">
         <v>0.01739130434782609</v>
@@ -41499,7 +41302,7 @@
         <v>1</v>
       </c>
       <c r="L14">
-        <v>0.9917355371900827</v>
+        <v>0.2396694214876033</v>
       </c>
       <c r="M14">
         <v>0.008264462809917356</v>
@@ -41698,7 +41501,7 @@
         <v>1</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="M15">
         <v>0.01388888888888889</v>
@@ -41897,7 +41700,7 @@
         <v>1</v>
       </c>
       <c r="L16">
-        <v>0.995</v>
+        <v>0.175</v>
       </c>
       <c r="M16">
         <v>0.02</v>
@@ -42096,7 +41899,7 @@
         <v>1</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>0.163716814159292</v>
       </c>
       <c r="M17">
         <v>0.008849557522123894</v>
@@ -42295,7 +42098,7 @@
         <v>1</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>0.1382113821138211</v>
       </c>
       <c r="M18">
         <v>0.008130081300813009</v>
@@ -42494,7 +42297,7 @@
         <v>1</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0.2030651340996169</v>
       </c>
       <c r="M19">
         <v>0.01149425287356322</v>
@@ -42693,7 +42496,7 @@
         <v>1</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0.136094674556213</v>
       </c>
       <c r="M20">
         <v>0.002958579881656805</v>
@@ -42892,7 +42695,7 @@
         <v>1</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0.1779448621553885</v>
       </c>
       <c r="M21">
         <v>0.007518796992481203</v>
@@ -43091,7 +42894,7 @@
         <v>1</v>
       </c>
       <c r="L22">
-        <v>0.9977973568281938</v>
+        <v>0.1277533039647577</v>
       </c>
       <c r="M22">
         <v>0.004405286343612335</v>
@@ -43290,7 +43093,7 @@
         <v>1</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>0.1705882352941177</v>
       </c>
       <c r="M23">
         <v>0.009803921568627451</v>
@@ -43489,7 +43292,7 @@
         <v>1</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>0.1436541143654114</v>
       </c>
       <c r="M24">
         <v>0.01673640167364017</v>
@@ -43688,7 +43491,7 @@
         <v>1</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>0.1729323308270677</v>
       </c>
       <c r="M25">
         <v>0.01353383458646617</v>
@@ -43887,7 +43690,7 @@
         <v>1</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0.1551724137931035</v>
       </c>
       <c r="M26">
         <v>0.01193633952254642</v>
@@ -44086,7 +43889,7 @@
         <v>1</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>0.1558784676354029</v>
       </c>
       <c r="M27">
         <v>0.01585204755614267</v>
@@ -44285,7 +44088,7 @@
         <v>1</v>
       </c>
       <c r="L28">
-        <v>0.9989035087719298</v>
+        <v>0.168859649122807</v>
       </c>
       <c r="M28">
         <v>0.008771929824561403</v>
@@ -44484,7 +44287,7 @@
         <v>1</v>
       </c>
       <c r="L29">
-        <v>0.9989429175475687</v>
+        <v>0.1469344608879493</v>
       </c>
       <c r="M29">
         <v>0.01691331923890063</v>
@@ -44683,7 +44486,7 @@
         <v>1</v>
       </c>
       <c r="L30">
-        <v>0.9990636704119851</v>
+        <v>0.1460674157303371</v>
       </c>
       <c r="M30">
         <v>0.02153558052434457</v>
@@ -44882,7 +44685,7 @@
         <v>1</v>
       </c>
       <c r="L31">
-        <v>1</v>
+        <v>0.1361702127659574</v>
       </c>
       <c r="M31">
         <v>0.01531914893617021</v>
@@ -45081,7 +44884,7 @@
         <v>1</v>
       </c>
       <c r="L32">
-        <v>0.9992727272727273</v>
+        <v>0.1418181818181818</v>
       </c>
       <c r="M32">
         <v>0.01381818181818182</v>
@@ -45280,7 +45083,7 @@
         <v>1</v>
       </c>
       <c r="L33">
-        <v>0.9986168741355463</v>
+        <v>0.1334716459197787</v>
       </c>
       <c r="M33">
         <v>0.01106500691562932</v>
@@ -45479,7 +45282,7 @@
         <v>1</v>
       </c>
       <c r="L34">
-        <v>0.9993585631815266</v>
+        <v>0.13662604233483</v>
       </c>
       <c r="M34">
         <v>0.01411161000641437</v>
@@ -45678,7 +45481,7 @@
         <v>1</v>
       </c>
       <c r="L35">
-        <v>1</v>
+        <v>0.138267355134825</v>
       </c>
       <c r="M35">
         <v>0.01032702237521515</v>
@@ -45877,7 +45680,7 @@
         <v>1</v>
       </c>
       <c r="L36">
-        <v>0.9994954591321897</v>
+        <v>0.127648839556004</v>
       </c>
       <c r="M36">
         <v>0.00958627648839556</v>
@@ -46076,7 +45879,7 @@
         <v>1</v>
       </c>
       <c r="L37">
-        <v>1</v>
+        <v>0.116921768707483</v>
       </c>
       <c r="M37">
         <v>0.01445578231292517</v>
@@ -46275,7 +46078,7 @@
         <v>1</v>
       </c>
       <c r="L38">
-        <v>1</v>
+        <v>0.1226343679031037</v>
       </c>
       <c r="M38">
         <v>0.01362604087812263</v>
@@ -46474,7 +46277,7 @@
         <v>1</v>
       </c>
       <c r="L39">
-        <v>0.9996713769306605</v>
+        <v>0.1189615511008873</v>
       </c>
       <c r="M39">
         <v>0.01840289188301019</v>
@@ -46673,7 +46476,7 @@
         <v>1</v>
       </c>
       <c r="L40">
-        <v>0.9995231282784931</v>
+        <v>0.09537434430138293</v>
       </c>
       <c r="M40">
         <v>0.01478302336671435</v>
@@ -46872,7 +46675,7 @@
         <v>1</v>
       </c>
       <c r="L41">
-        <v>0.9992082343626286</v>
+        <v>0.09699129057798891</v>
       </c>
       <c r="M41">
         <v>0.01543942992874109</v>
@@ -47071,7 +46874,7 @@
         <v>1</v>
       </c>
       <c r="L42">
-        <v>1</v>
+        <v>0.09006066262249184</v>
       </c>
       <c r="M42">
         <v>0.01726551563229118</v>
@@ -47270,7 +47073,7 @@
         <v>1</v>
       </c>
       <c r="L43">
-        <v>0.9994797086368367</v>
+        <v>0.1030176899063475</v>
       </c>
       <c r="M43">
         <v>0.0145681581685744</v>
@@ -47469,7 +47272,7 @@
         <v>1</v>
       </c>
       <c r="L44">
-        <v>1</v>
+        <v>0.08772969768820391</v>
       </c>
       <c r="M44">
         <v>0.01837581505631298</v>
@@ -47668,7 +47471,7 @@
         <v>1</v>
       </c>
       <c r="L45">
-        <v>0.9993145990404386</v>
+        <v>0.09184372858122002</v>
       </c>
       <c r="M45">
         <v>0.01713502398903358</v>
@@ -47867,7 +47670,7 @@
         <v>1</v>
       </c>
       <c r="L46">
-        <v>0.998472116119175</v>
+        <v>0.07715813598166539</v>
       </c>
       <c r="M46">
         <v>0.009167303284950344</v>
@@ -48066,7 +47869,7 @@
         <v>1</v>
       </c>
       <c r="L47">
-        <v>1</v>
+        <v>0.08467023172905526</v>
       </c>
       <c r="M47">
         <v>0.02228163992869875</v>
@@ -48265,7 +48068,7 @@
         <v>1</v>
       </c>
       <c r="L48">
-        <v>0.999074502545118</v>
+        <v>0.06478482184173993</v>
       </c>
       <c r="M48">
         <v>0.01804720037019898</v>
@@ -48464,7 +48267,7 @@
         <v>1</v>
       </c>
       <c r="L49">
-        <v>0.9859154929577465</v>
+        <v>0.09859154929577464</v>
       </c>
       <c r="M49">
         <v>0.04225352112676056</v>
@@ -48663,7 +48466,7 @@
         <v>1</v>
       </c>
       <c r="L50">
-        <v>1</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="M50">
         <v>0.04545454545454546</v>
@@ -49396,7 +49199,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.999292202430105</v>
+        <v>0.07207738586764185</v>
       </c>
       <c r="M2">
         <v>0.01922850064881444</v>
@@ -49595,7 +49398,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9994520547945206</v>
+        <v>0.1303013698630137</v>
       </c>
       <c r="M3">
         <v>0.01802739726027397</v>
@@ -49794,7 +49597,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9993462628023535</v>
+        <v>0.2020047940727827</v>
       </c>
       <c r="M4">
         <v>0.01765090433645674</v>
@@ -49993,7 +49796,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9988088147706968</v>
+        <v>0.2412150089338892</v>
       </c>
       <c r="M5">
         <v>0.01310303752233472</v>
@@ -50724,7 +50527,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994586303347469</v>
+        <v>0.1166200487232699</v>
       </c>
       <c r="M2">
         <v>0.0150455652801588</v>
@@ -50921,7 +50724,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9992435703479576</v>
+        <v>0.1944024205748865</v>
       </c>
       <c r="M3">
         <v>0.00226928895612708</v>
@@ -51460,7 +51263,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995189995189995</v>
+        <v>0.09716209716209716</v>
       </c>
       <c r="M2">
         <v>0.02573352573352573</v>
@@ -51659,7 +51462,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.999540018399264</v>
+        <v>0.1056117755289788</v>
       </c>
       <c r="M3">
         <v>0.01830726770929163</v>
@@ -51858,7 +51661,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0.112972972972973</v>
       </c>
       <c r="M4">
         <v>0.005405405405405406</v>
@@ -52057,7 +51860,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9994169096209913</v>
+        <v>0.124198250728863</v>
       </c>
       <c r="M5">
         <v>0.01341107871720117</v>
@@ -52256,7 +52059,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9991315675206253</v>
+        <v>0.1214358083658996</v>
       </c>
       <c r="M6">
         <v>0.01432913590968302</v>
@@ -52455,7 +52258,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.9991060253888789</v>
+        <v>0.1298051135347756</v>
       </c>
       <c r="M7">
         <v>0.01180046486679778</v>
@@ -52654,7 +52457,7 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0.141390205371248</v>
       </c>
       <c r="M8">
         <v>0.01145339652448657</v>
@@ -52853,7 +52656,7 @@
         <v>1</v>
       </c>
       <c r="L9">
-        <v>0.9993734335839599</v>
+        <v>0.1397243107769424</v>
       </c>
       <c r="M9">
         <v>0.009398496240601503</v>
@@ -53052,7 +52855,7 @@
         <v>1</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>0.1384083044982699</v>
       </c>
       <c r="M10">
         <v>0.01384083044982699</v>
@@ -53251,7 +53054,7 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0.1485148514851485</v>
       </c>
       <c r="M11">
         <v>0.006600660066006601</v>
@@ -53450,7 +53253,7 @@
         <v>1</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0.1636363636363636</v>
       </c>
       <c r="M12">
         <v>0.006060606060606061</v>
@@ -54181,7 +53984,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9996135713733674</v>
+        <v>0.1037174433882062</v>
       </c>
       <c r="M2">
         <v>0.01290671612953088</v>
@@ -54378,7 +54181,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9993693783398055</v>
+        <v>0.1245311825815659</v>
       </c>
       <c r="M3">
         <v>0.01573235089116798</v>
@@ -55109,7 +54912,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994223826714801</v>
+        <v>0.06216606498194946</v>
       </c>
       <c r="M2">
         <v>0.01436823104693141</v>
@@ -55306,7 +55109,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.998</v>
+        <v>0.138</v>
       </c>
       <c r="M3">
         <v>0.022</v>
@@ -55503,7 +55306,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9994619316653215</v>
+        <v>0.161151466236212</v>
       </c>
       <c r="M4">
         <v>0.01049233252623083</v>
@@ -55700,7 +55503,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0.09846547314578005</v>
       </c>
       <c r="M5">
         <v>0.02088661551577153</v>
@@ -55897,7 +55700,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9996515679442509</v>
+        <v>0.08850174216027874</v>
       </c>
       <c r="M6">
         <v>0.01986062717770035</v>
@@ -56094,7 +55897,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.08148148148148149</v>
       </c>
       <c r="M7">
         <v>0.02962962962962963</v>
@@ -56291,7 +56094,7 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0.1636363636363636</v>
       </c>
       <c r="M8">
         <v>0.03636363636363636</v>
@@ -56488,7 +56291,7 @@
         <v>1</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0.1641791044776119</v>
       </c>
       <c r="M9">
         <v>0.02985074626865672</v>
@@ -56685,7 +56488,7 @@
         <v>1</v>
       </c>
       <c r="L10">
-        <v>0.9994849463876012</v>
+        <v>0.1546565528866414</v>
       </c>
       <c r="M10">
         <v>0.01428103198014702</v>
@@ -57416,7 +57219,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994509265614276</v>
+        <v>0.1547014413177762</v>
       </c>
       <c r="M2">
         <v>0.01455044612216884</v>
@@ -57613,7 +57416,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9995677120176059</v>
+        <v>0.1175823312111923</v>
       </c>
       <c r="M3">
         <v>0.0148942859388509</v>
@@ -58346,7 +58149,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994788582257491</v>
+        <v>0.1227288878360772</v>
       </c>
       <c r="M2">
         <v>0.01444984010422836</v>
@@ -58545,7 +58348,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9991192014092778</v>
+        <v>0.07134468584850265</v>
       </c>
       <c r="M3">
         <v>0.01702877275396359</v>
@@ -59276,7 +59079,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994485560876506</v>
+        <v>0.0983601799448556</v>
       </c>
       <c r="M2">
         <v>0.01622406036859672</v>
@@ -59473,7 +59276,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9994275901545506</v>
+        <v>0.2192329708070979</v>
       </c>
       <c r="M3">
         <v>0.01058958214081282</v>
@@ -60204,7 +60007,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994367307854789</v>
+        <v>0.09907905483425804</v>
       </c>
       <c r="M2">
         <v>0.01582786492804236</v>
@@ -60401,7 +60204,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9994958830448664</v>
+        <v>0.1557721391362796</v>
       </c>
       <c r="M3">
         <v>0.01193076793816165</v>
@@ -60598,7 +60401,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9996260284218399</v>
+        <v>0.2097980553477936</v>
       </c>
       <c r="M4">
         <v>0.009349289454001496</v>
@@ -60795,7 +60598,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9990645463049579</v>
+        <v>0.2619270346117867</v>
       </c>
       <c r="M5">
         <v>0.01122544434050514</v>
@@ -60992,7 +60795,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.3220858895705521</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -61189,7 +60992,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.2909090909090909</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -61386,7 +61189,7 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -61923,7 +61726,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994485560876506</v>
+        <v>0.0983601799448556</v>
       </c>
       <c r="M2">
         <v>0.01622406036859672</v>
@@ -62120,7 +61923,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9997058390939844</v>
+        <v>0.1975290483894691</v>
       </c>
       <c r="M3">
         <v>0.009854390351522283</v>
@@ -62851,7 +62654,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994485560876506</v>
+        <v>0.0983601799448556</v>
       </c>
       <c r="M2">
         <v>0.01622406036859672</v>
@@ -63048,7 +62851,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.2443384982121573</v>
       </c>
       <c r="M3">
         <v>0.01072705601907032</v>
@@ -63779,7 +63582,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994485560876506</v>
+        <v>0.0983601799448556</v>
       </c>
       <c r="M2">
         <v>0.01622406036859672</v>
@@ -63976,7 +63779,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9993573264781491</v>
+        <v>0.2506426735218509</v>
       </c>
       <c r="M3">
         <v>0.0102827763496144</v>
@@ -64707,7 +64510,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994485560876506</v>
+        <v>0.0983601799448556</v>
       </c>
       <c r="M2">
         <v>0.01622406036859672</v>
@@ -64904,7 +64707,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9996637525218561</v>
+        <v>0.2057834566240753</v>
       </c>
       <c r="M3">
         <v>0.006388702084734364</v>
@@ -65637,7 +65440,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9993557392891657</v>
+        <v>0.1226242886287985</v>
       </c>
       <c r="M2">
         <v>0.01790507892193708</v>
@@ -65836,7 +65639,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9998805542283803</v>
+        <v>0.1021261347348304</v>
       </c>
       <c r="M3">
         <v>0.000358337314859054</v>
@@ -66567,7 +66370,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9990639625585024</v>
+        <v>0.1274570982839314</v>
       </c>
       <c r="M2">
         <v>0.01029641185647426</v>
@@ -66764,7 +66567,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9995373048004627</v>
+        <v>0.1338345864661654</v>
       </c>
       <c r="M3">
         <v>0.01075766338924234</v>
@@ -66961,7 +66764,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9996529384544193</v>
+        <v>0.1316520129569644</v>
       </c>
       <c r="M4">
         <v>0.01550208236927348</v>
@@ -67158,7 +66961,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9992898567877856</v>
+        <v>0.1371759971594272</v>
       </c>
       <c r="M5">
         <v>0.01657000828500414</v>
@@ -67355,7 +67158,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.999618320610687</v>
+        <v>0.1061068702290076</v>
       </c>
       <c r="M6">
         <v>0.01717557251908397</v>
@@ -67552,7 +67355,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.9993900579444953</v>
+        <v>0.08234217749313816</v>
       </c>
       <c r="M7">
         <v>0.02317779810917963</v>
@@ -67749,7 +67552,7 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>0.9996209249431387</v>
+        <v>0.0667172100075815</v>
       </c>
       <c r="M8">
         <v>0.01364670204700531</v>
@@ -67946,7 +67749,7 @@
         <v>1</v>
       </c>
       <c r="L9">
-        <v>0.9995742869306088</v>
+        <v>0.06555981268624947</v>
       </c>
       <c r="M9">
         <v>0.01489995742869306</v>
@@ -68485,7 +68288,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9988246816846229</v>
+        <v>0.2268364348677767</v>
       </c>
       <c r="M2">
         <v>0.01155729676787463</v>
@@ -68684,7 +68487,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9994698710019438</v>
+        <v>0.1816575366672557</v>
       </c>
       <c r="M3">
         <v>0.01466690227955469</v>
@@ -68883,7 +68686,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9996100857811282</v>
+        <v>0.1460878606706525</v>
       </c>
       <c r="M4">
         <v>0.01364699766051469</v>
@@ -69082,7 +68885,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9996793844180827</v>
+        <v>0.1356203911510099</v>
       </c>
       <c r="M5">
         <v>0.01058031420327028</v>
@@ -69281,7 +69084,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9993999399939995</v>
+        <v>0.1296129612961296</v>
       </c>
       <c r="M6">
         <v>0.0138013801380138</v>
@@ -69480,7 +69283,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.12348401323043</v>
       </c>
       <c r="M7">
         <v>0.01984564498346196</v>
@@ -70213,7 +70016,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994695609596866</v>
+        <v>0.1033132038518035</v>
       </c>
       <c r="M2">
         <v>0.01640280724661335</v>
@@ -70412,7 +70215,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9995544002970664</v>
+        <v>0.122020051986632</v>
       </c>
       <c r="M3">
         <v>0.01477905681396212</v>
@@ -70611,7 +70414,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9990961677512654</v>
+        <v>0.1576283441793203</v>
       </c>
       <c r="M4">
         <v>0.008857556037599421</v>
@@ -70810,7 +70613,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9991055456171736</v>
+        <v>0.1735241502683363</v>
       </c>
       <c r="M5">
         <v>0.007155635062611807</v>
@@ -71009,7 +70812,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.1951219512195122</v>
       </c>
       <c r="M6">
         <v>0.01219512195121951</v>
@@ -71208,7 +71011,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.2178988326848249</v>
       </c>
       <c r="M7">
         <v>0.01945525291828794</v>
@@ -71939,7 +71742,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995093009769371</v>
+        <v>0.1169648034973458</v>
       </c>
       <c r="M2">
         <v>0.01474327519293393</v>
@@ -72136,7 +71939,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.2996031746031746</v>
       </c>
       <c r="M3">
         <v>0.01785714285714286</v>
@@ -72869,7 +72672,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9989733059548255</v>
+        <v>0.1047227926078029</v>
       </c>
       <c r="M2">
         <v>0.02019164955509925</v>
@@ -73068,7 +72871,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.1830188679245283</v>
       </c>
       <c r="M3">
         <v>0.003773584905660377</v>
@@ -73267,7 +73070,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.999443052074631</v>
+        <v>0.0847953216374269</v>
       </c>
       <c r="M4">
         <v>0.01559454191033138</v>
@@ -73466,7 +73269,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9991532599491956</v>
+        <v>0.1215071972904318</v>
       </c>
       <c r="M5">
         <v>0.02074513124470788</v>
@@ -73665,7 +73468,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.1575757575757576</v>
       </c>
       <c r="M6">
         <v>0.01212121212121212</v>
@@ -73864,7 +73667,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.1070234113712375</v>
       </c>
       <c r="M7">
         <v>0.01114827201783724</v>
@@ -74063,7 +73866,7 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>0.9995159896283492</v>
+        <v>0.1272255834053587</v>
       </c>
       <c r="M8">
         <v>0.01334485738980121</v>
@@ -74262,7 +74065,7 @@
         <v>1</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0.1452513966480447</v>
       </c>
       <c r="M9">
         <v>0.00558659217877095</v>
@@ -74461,7 +74264,7 @@
         <v>1</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>0.08860759493670886</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -75194,7 +74997,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9997170745508559</v>
+        <v>0.08020936483236667</v>
       </c>
       <c r="M2">
         <v>0.01980478144009054</v>
@@ -75393,7 +75196,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9995779700358726</v>
+        <v>0.118062882464655</v>
       </c>
       <c r="M3">
         <v>0.01466554125342899</v>
@@ -75592,7 +75395,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9994681322577785</v>
+        <v>0.1226841592057442</v>
       </c>
       <c r="M4">
         <v>0.0150695860296073</v>
@@ -75791,7 +75594,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9989424206815511</v>
+        <v>0.1340775558166863</v>
       </c>
       <c r="M5">
         <v>0.01257344300822562</v>
@@ -75990,7 +75793,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9995706311721769</v>
+        <v>0.1305281236582224</v>
       </c>
       <c r="M6">
         <v>0.01223701159295835</v>
@@ -76529,7 +76332,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9993512812195913</v>
+        <v>0.1279922153746351</v>
       </c>
       <c r="M2">
         <v>0.01037950048653908</v>
@@ -76728,7 +76531,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.1198246468582562</v>
       </c>
       <c r="M3">
         <v>0.006332196785192402</v>
@@ -76927,7 +76730,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0.1413533834586466</v>
       </c>
       <c r="M4">
         <v>0.009022556390977444</v>
@@ -77126,7 +76929,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0.1201923076923077</v>
       </c>
       <c r="M5">
         <v>0.02243589743589744</v>
@@ -77325,7 +77128,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9993767205110892</v>
+        <v>0.117851763361554</v>
       </c>
       <c r="M6">
         <v>0.01958136394328156</v>
@@ -77524,7 +77327,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.9996138996138996</v>
+        <v>0.08957528957528957</v>
       </c>
       <c r="M7">
         <v>0.01621621621621622</v>
@@ -77723,7 +77526,7 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>0.9974937343358395</v>
+        <v>0.1453634085213033</v>
       </c>
       <c r="M8">
         <v>0.007518796992481203</v>
@@ -78456,7 +78259,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995941146626078</v>
+        <v>0.1066463723997971</v>
       </c>
       <c r="M2">
         <v>0.0008117706747843734</v>
@@ -78655,7 +78458,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9993552546744036</v>
+        <v>0.1553836234687299</v>
       </c>
       <c r="M3">
         <v>0.01289490651192779</v>
@@ -78854,7 +78657,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9997095556200988</v>
+        <v>0.1417368573918095</v>
       </c>
       <c r="M4">
         <v>0.01975021783328493</v>
@@ -79053,7 +78856,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.99942502299908</v>
+        <v>0.1294848206071757</v>
       </c>
       <c r="M5">
         <v>0.01655933762649494</v>
@@ -79252,7 +79055,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9994158196050941</v>
+        <v>0.1174202593760953</v>
       </c>
       <c r="M6">
         <v>0.01910269891342447</v>
@@ -79451,7 +79254,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.999189134400973</v>
+        <v>0.1023717818771539</v>
       </c>
       <c r="M7">
         <v>0.02067707277518751</v>
@@ -80184,7 +79987,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.999475485176212</v>
+        <v>0.1155680995079551</v>
       </c>
       <c r="M2">
         <v>0.01673452056847416</v>
@@ -80383,7 +80186,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9988304093567252</v>
+        <v>0.1052631578947368</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -80582,7 +80385,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9991944146079484</v>
+        <v>0.1498388829215897</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -81315,7 +81118,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995020471395375</v>
+        <v>0.09895429899302866</v>
       </c>
       <c r="M2">
         <v>0.01637711629965697</v>
@@ -81514,7 +81317,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.1386263390044108</v>
       </c>
       <c r="M3">
         <v>0.01071203528670447</v>
@@ -81713,7 +81516,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9995069033530573</v>
+        <v>0.2186883629191322</v>
       </c>
       <c r="M4">
         <v>0.009615384615384616</v>
@@ -81912,7 +81715,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9988434849653045</v>
+        <v>0.1981495759444873</v>
       </c>
       <c r="M5">
         <v>0.004626060138781804</v>
@@ -82111,7 +81914,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9991379310344828</v>
+        <v>0.1844827586206897</v>
       </c>
       <c r="M6">
         <v>0.006896551724137931</v>
@@ -82310,7 +82113,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.9908256880733946</v>
+        <v>0.1376146788990826</v>
       </c>
       <c r="M7">
         <v>0.01834862385321101</v>
@@ -82849,7 +82652,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9994290499390986</v>
+        <v>0.09264616321559074</v>
       </c>
       <c r="M2">
         <v>0.02044001218026796</v>
@@ -83048,7 +82851,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9995606326889279</v>
+        <v>0.1963971880492091</v>
       </c>
       <c r="M3">
         <v>0.01340070298769772</v>
@@ -83247,7 +83050,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0.2408182240818224</v>
       </c>
       <c r="M4">
         <v>0.01208740120874012</v>
@@ -83446,7 +83249,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9990272373540856</v>
+        <v>0.2655642023346304</v>
       </c>
       <c r="M5">
         <v>0.008754863813229572</v>
@@ -83645,7 +83448,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9959432048681541</v>
+        <v>0.2210953346855984</v>
       </c>
       <c r="M6">
         <v>0.01622718052738337</v>
@@ -83844,7 +83647,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.215</v>
       </c>
       <c r="M7">
         <v>0.03</v>
@@ -84043,7 +83846,7 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -84774,7 +84577,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9993686449126071</v>
+        <v>0.1133780820097029</v>
       </c>
       <c r="M2">
         <v>0.0187080481159035</v>
@@ -84971,7 +84774,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9998214604534904</v>
+        <v>0.1787180860560614</v>
       </c>
       <c r="M3">
         <v>0.01731833601142653</v>
@@ -85704,7 +85507,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9997363564460849</v>
+        <v>0.1270761929870815</v>
       </c>
       <c r="M2">
         <v>0.005272871078302136</v>
@@ -85903,7 +85706,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9991956565453448</v>
+        <v>0.1145183993565252</v>
       </c>
       <c r="M3">
         <v>0.005932032978081641</v>
@@ -86102,7 +85905,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9994390688542981</v>
+        <v>0.1128873930725004</v>
       </c>
       <c r="M4">
         <v>0.00448744916561492</v>
@@ -86301,7 +86104,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0.1143625967036663</v>
       </c>
       <c r="M5">
         <v>0.006054490413723511</v>
@@ -86500,7 +86303,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.1462686567164179</v>
       </c>
       <c r="M6">
         <v>0.004975124378109453</v>
@@ -86699,7 +86502,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.1840277777777778</v>
       </c>
       <c r="M7">
         <v>0.003472222222222222</v>
@@ -87432,7 +87235,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0.162109375</v>
       </c>
       <c r="M2">
         <v>0.00390625</v>
@@ -87631,7 +87434,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.1277509393451423</v>
       </c>
       <c r="M3">
         <v>0.005636070853462158</v>
@@ -87830,7 +87633,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9995645231528524</v>
+        <v>0.1136594571055306</v>
       </c>
       <c r="M4">
         <v>0.006386993758165191</v>
@@ -88029,7 +87832,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9992386752950133</v>
+        <v>0.1164826798629616</v>
       </c>
       <c r="M5">
         <v>0.005329272934906737</v>
@@ -88228,7 +88031,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9995040502562407</v>
+        <v>0.1153909737146636</v>
       </c>
       <c r="M6">
         <v>0.004132914531327492</v>
@@ -88427,7 +88230,7 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.9990825688073395</v>
+        <v>0.1045871559633028</v>
       </c>
       <c r="M7">
         <v>0.005963302752293578</v>
@@ -89160,7 +88963,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9990297542043984</v>
+        <v>0.1177231565329884</v>
       </c>
       <c r="M2">
         <v>0.01196636481241915</v>
@@ -89359,7 +89162,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.1297071129707113</v>
       </c>
       <c r="M3">
         <v>0.01135684399282726</v>
@@ -89558,7 +89361,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9995144131020174</v>
+        <v>0.1069615503465325</v>
       </c>
       <c r="M4">
         <v>0.01390544298768375</v>
@@ -89757,7 +89560,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.9994974874371859</v>
+        <v>0.1336683417085427</v>
       </c>
       <c r="M5">
         <v>0.01669458403126745</v>
@@ -90488,7 +90291,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995649651972158</v>
+        <v>0.1351508120649652</v>
       </c>
       <c r="M2">
         <v>0.01334106728538283</v>
@@ -90685,7 +90488,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9990721410345628</v>
+        <v>0.1762932034330782</v>
       </c>
       <c r="M3">
         <v>0.01322199025748086</v>
@@ -90882,7 +90685,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.99963530269876</v>
+        <v>0.1830780452224653</v>
       </c>
       <c r="M4">
         <v>0.01239970824215901</v>
@@ -91079,7 +90882,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0.1861240827218145</v>
       </c>
       <c r="M5">
         <v>0.01734489659773182</v>
@@ -91276,7 +91079,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9994794377928162</v>
+        <v>0.2131702238417491</v>
       </c>
       <c r="M6">
         <v>0.009630400832899531</v>
@@ -92007,7 +91810,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995326738842589</v>
+        <v>0.116987304307189</v>
       </c>
       <c r="M2">
         <v>0.01838149388581665</v>
@@ -92204,7 +92007,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9993874693734687</v>
+        <v>0.1273626181309065</v>
       </c>
       <c r="M3">
         <v>0.01855092754637732</v>
@@ -92937,7 +92740,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9995096342448367</v>
+        <v>0.0854678666205146</v>
       </c>
       <c r="M2">
         <v>0.01427829698857736</v>
@@ -93136,7 +92939,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9992718004733296</v>
+        <v>0.2242854542144548</v>
       </c>
       <c r="M3">
         <v>0.01592936464591298</v>
@@ -93675,7 +93478,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.999515403253721</v>
+        <v>0.1078573901003808</v>
       </c>
       <c r="M2">
         <v>0.01479173877927772</v>
@@ -93874,7 +93677,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9982751185855973</v>
+        <v>0.3247089262613195</v>
       </c>
       <c r="M3">
         <v>0.01250539025442001</v>

</xml_diff>